<commit_message>
single rail amp, themistor voltage readout
</commit_message>
<xml_diff>
--- a/pcb/bom.xlsx
+++ b/pcb/bom.xlsx
@@ -452,18 +452,6 @@
     <t>490-10018-1-ND</t>
   </si>
   <si>
-    <t>CAP CER 0.1UF 10V X5R 0402</t>
-  </si>
-  <si>
-    <t>CL05A104KP5NNNC</t>
-  </si>
-  <si>
-    <t>1276-1022-1-ND</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-detail/en/CL05A104KP5NNNC/1276-1022-1-ND/3889108</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-detail/en/BAV103-GS18/BAV103-GS18CT-ND/3104430</t>
   </si>
   <si>
@@ -546,6 +534,18 @@
   </si>
   <si>
     <t>160-1475-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 100V X5R 0402</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/GRM155R62A104ME14D/490-10459-1-ND/5026371</t>
+  </si>
+  <si>
+    <t>GRM155R62A104ME14D</t>
+  </si>
+  <si>
+    <t>490-10459-1-ND</t>
   </si>
 </sst>
 </file>
@@ -554,7 +554,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -599,7 +599,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -883,7 +883,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1055,26 +1057,26 @@
         <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>141</v>
+        <v>169</v>
       </c>
       <c r="D6" t="s">
-        <v>142</v>
+        <v>171</v>
       </c>
       <c r="E6" t="s">
-        <v>143</v>
+        <v>172</v>
       </c>
       <c r="F6" s="3">
         <v>4</v>
       </c>
       <c r="G6" s="5">
-        <v>4.7999999999999996E-3</v>
+        <v>1.1599999999999999E-2</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
-        <v>1.9199999999999998E-2</v>
+        <v>4.6399999999999997E-2</v>
       </c>
       <c r="I6" t="s">
-        <v>144</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1097,7 +1099,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="1">
-        <f>G7*F7</f>
+        <f t="shared" ref="H7:H30" si="2">G7*F7</f>
         <v>0</v>
       </c>
     </row>
@@ -1109,13 +1111,13 @@
         <v>109</v>
       </c>
       <c r="C8" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D8" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E8" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F8" s="4">
         <v>1</v>
@@ -1124,11 +1126,11 @@
         <v>0.24</v>
       </c>
       <c r="H8" s="1">
-        <f>G8*F8</f>
+        <f t="shared" si="2"/>
         <v>0.24</v>
       </c>
       <c r="I8" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1139,13 +1141,13 @@
         <v>94</v>
       </c>
       <c r="C9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D9" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F9" s="4">
         <v>1</v>
@@ -1154,11 +1156,11 @@
         <v>0.19</v>
       </c>
       <c r="H9" s="1">
-        <f>G9*F9</f>
+        <f t="shared" si="2"/>
         <v>0.19</v>
       </c>
       <c r="I9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1169,13 +1171,13 @@
         <v>76</v>
       </c>
       <c r="C10" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D10" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E10" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F10" s="4">
         <v>1</v>
@@ -1184,11 +1186,11 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="H10" s="1">
-        <f>G10*F10</f>
+        <f t="shared" si="2"/>
         <v>0.56999999999999995</v>
       </c>
       <c r="I10" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1214,7 +1216,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="1">
-        <f>G11*F11</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I11" t="s">
@@ -1229,13 +1231,13 @@
         <v>78</v>
       </c>
       <c r="C12" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D12" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E12" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F12" s="4">
         <v>1</v>
@@ -1244,11 +1246,11 @@
         <v>1.71</v>
       </c>
       <c r="H12" s="1">
-        <f>G12*F12</f>
+        <f t="shared" si="2"/>
         <v>1.71</v>
       </c>
       <c r="I12" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1274,11 +1276,11 @@
         <v>0</v>
       </c>
       <c r="H13" s="1">
-        <f>G13*F13</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1289,13 +1291,13 @@
         <v>90</v>
       </c>
       <c r="C14" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D14" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E14" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F14" s="4">
         <v>1</v>
@@ -1304,11 +1306,11 @@
         <v>0.45</v>
       </c>
       <c r="H14" s="1">
-        <f>G14*F14</f>
+        <f t="shared" si="2"/>
         <v>0.45</v>
       </c>
       <c r="I14" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1334,7 +1336,7 @@
         <v>0.94</v>
       </c>
       <c r="H15" s="1">
-        <f>G15*F15</f>
+        <f t="shared" si="2"/>
         <v>0.94</v>
       </c>
       <c r="I15" t="s">
@@ -1349,13 +1351,13 @@
         <v>74</v>
       </c>
       <c r="C16" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D16" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E16" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F16" s="4">
         <v>1</v>
@@ -1364,11 +1366,11 @@
         <v>0.86</v>
       </c>
       <c r="H16" s="1">
-        <f>G16*F16</f>
+        <f t="shared" si="2"/>
         <v>0.86</v>
       </c>
       <c r="I16" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1394,7 +1396,7 @@
         <v>0</v>
       </c>
       <c r="H17" s="1">
-        <f>G17*F17</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I17" t="s">
@@ -1424,7 +1426,7 @@
         <v>0.38</v>
       </c>
       <c r="H18" s="1">
-        <f>G18*F18</f>
+        <f t="shared" si="2"/>
         <v>0.76</v>
       </c>
       <c r="I18" t="s">
@@ -1454,7 +1456,7 @@
         <v>0.5</v>
       </c>
       <c r="H19" s="1">
-        <f>G19*F19</f>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="I19" t="s">
@@ -1484,7 +1486,7 @@
         <v>0.38</v>
       </c>
       <c r="H20" s="1">
-        <f>G20*F20</f>
+        <f t="shared" si="2"/>
         <v>1.9</v>
       </c>
       <c r="I20" t="s">
@@ -1514,7 +1516,7 @@
         <v>0.7</v>
       </c>
       <c r="H21" s="1">
-        <f>G21*F21</f>
+        <f t="shared" si="2"/>
         <v>0.7</v>
       </c>
       <c r="I21" t="s">
@@ -1544,7 +1546,7 @@
         <v>4.7000000000000002E-3</v>
       </c>
       <c r="H22" s="1">
-        <f>G22*F22</f>
+        <f t="shared" si="2"/>
         <v>2.35E-2</v>
       </c>
       <c r="I22" t="s">
@@ -1574,7 +1576,7 @@
         <v>0.4</v>
       </c>
       <c r="H23" s="1">
-        <f>G23*F23</f>
+        <f t="shared" si="2"/>
         <v>0.4</v>
       </c>
       <c r="I23" t="s">
@@ -1604,7 +1606,7 @@
         <v>0.4</v>
       </c>
       <c r="H24" s="1">
-        <f>G24*F24</f>
+        <f t="shared" si="2"/>
         <v>0.4</v>
       </c>
       <c r="I24" t="s">
@@ -1634,7 +1636,7 @@
         <v>4.7000000000000002E-3</v>
       </c>
       <c r="H25" s="1">
-        <f>G25*F25</f>
+        <f t="shared" si="2"/>
         <v>1.4100000000000001E-2</v>
       </c>
       <c r="I25" t="s">
@@ -1664,7 +1666,7 @@
         <v>4.7000000000000002E-3</v>
       </c>
       <c r="H26" s="1">
-        <f>G26*F26</f>
+        <f t="shared" si="2"/>
         <v>9.4000000000000004E-3</v>
       </c>
       <c r="I26" t="s">
@@ -1694,7 +1696,7 @@
         <v>5.51</v>
       </c>
       <c r="H27" s="1">
-        <f>G27*F27</f>
+        <f t="shared" si="2"/>
         <v>5.51</v>
       </c>
       <c r="I27" t="s">
@@ -1709,13 +1711,13 @@
         <v>108</v>
       </c>
       <c r="C28" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D28" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E28" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F28" s="4">
         <v>1</v>
@@ -1724,11 +1726,11 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="H28" s="1">
-        <f>G28*F28</f>
+        <f t="shared" si="2"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="I28" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1754,7 +1756,7 @@
         <v>5.21</v>
       </c>
       <c r="H29" s="1">
-        <f>G29*F29</f>
+        <f t="shared" si="2"/>
         <v>5.21</v>
       </c>
       <c r="I29" t="s">
@@ -1784,7 +1786,7 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="H30" s="1">
-        <f>G30*F30</f>
+        <f t="shared" si="2"/>
         <v>1.1299999999999999</v>
       </c>
       <c r="I30" t="s">

</xml_diff>

<commit_message>
Fixed BOM errors, pcb approx postioning/sizing done
</commit_message>
<xml_diff>
--- a/pcb/bom.xlsx
+++ b/pcb/bom.xlsx
@@ -83,9 +83,6 @@
     <t>Op-Amp Power</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-detail/en/TPS65133DPDR/296-40874-1-ND/5178751</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-detail/en/LM94021BIMG%2FNOPB/LM94021BIMG%2FNOPBCT-ND/755138</t>
   </si>
   <si>
@@ -546,6 +543,9 @@
   </si>
   <si>
     <t>490-10459-1-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/PDS1-S5-D5-M-TR/102-3330-1-ND/4841469</t>
   </si>
 </sst>
 </file>
@@ -884,7 +884,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,12 +897,12 @@
     <col min="6" max="6" width="8.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="90.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -931,19 +931,19 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
         <v>39</v>
       </c>
-      <c r="B2" t="s">
-        <v>40</v>
-      </c>
       <c r="C2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D2" t="s">
         <v>131</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>132</v>
-      </c>
-      <c r="E2" t="s">
-        <v>133</v>
       </c>
       <c r="F2" s="3">
         <v>2</v>
@@ -956,24 +956,24 @@
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="I2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
         <v>43</v>
       </c>
-      <c r="B3" t="s">
-        <v>44</v>
-      </c>
       <c r="C3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" t="s">
         <v>134</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>135</v>
-      </c>
-      <c r="E3" t="s">
-        <v>136</v>
       </c>
       <c r="F3" s="3">
         <v>1</v>
@@ -986,24 +986,24 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="I3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" t="s">
         <v>50</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>51</v>
-      </c>
-      <c r="E4" t="s">
-        <v>52</v>
       </c>
       <c r="F4" s="3">
         <v>1</v>
@@ -1016,24 +1016,24 @@
         <v>3.61</v>
       </c>
       <c r="I4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E5" t="s">
         <v>139</v>
-      </c>
-      <c r="E5" t="s">
-        <v>140</v>
       </c>
       <c r="F5" s="3">
         <v>2</v>
@@ -1046,24 +1046,24 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="I5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
         <v>41</v>
       </c>
-      <c r="B6" t="s">
-        <v>42</v>
-      </c>
       <c r="C6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D6" t="s">
+        <v>170</v>
+      </c>
+      <c r="E6" t="s">
         <v>171</v>
-      </c>
-      <c r="E6" t="s">
-        <v>172</v>
       </c>
       <c r="F6" s="3">
         <v>4</v>
@@ -1076,24 +1076,24 @@
         <v>4.6399999999999997E-2</v>
       </c>
       <c r="I6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
         <v>37</v>
       </c>
-      <c r="B7" t="s">
-        <v>38</v>
-      </c>
       <c r="C7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" t="s">
         <v>48</v>
       </c>
-      <c r="D7" t="s">
-        <v>49</v>
-      </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7" s="3">
         <v>1</v>
@@ -1105,19 +1105,19 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" t="s">
         <v>166</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>167</v>
-      </c>
-      <c r="E8" t="s">
-        <v>168</v>
       </c>
       <c r="F8" s="4">
         <v>1</v>
@@ -1130,24 +1130,24 @@
         <v>0.24</v>
       </c>
       <c r="I8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E9" t="s">
         <v>142</v>
-      </c>
-      <c r="D9" t="s">
-        <v>144</v>
-      </c>
-      <c r="E9" t="s">
-        <v>143</v>
       </c>
       <c r="F9" s="4">
         <v>1</v>
@@ -1160,24 +1160,24 @@
         <v>0.19</v>
       </c>
       <c r="I9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" t="s">
         <v>75</v>
       </c>
-      <c r="B10" t="s">
-        <v>76</v>
-      </c>
       <c r="C10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D10" t="s">
         <v>146</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>147</v>
-      </c>
-      <c r="E10" t="s">
-        <v>148</v>
       </c>
       <c r="F10" s="4">
         <v>1</v>
@@ -1190,24 +1190,24 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="I10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" t="s">
         <v>54</v>
       </c>
-      <c r="D11" t="s">
-        <v>55</v>
-      </c>
       <c r="E11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F11" s="3">
         <v>1</v>
@@ -1220,24 +1220,24 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" t="s">
         <v>77</v>
       </c>
-      <c r="B12" t="s">
-        <v>78</v>
-      </c>
       <c r="C12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D12" t="s">
+        <v>149</v>
+      </c>
+      <c r="E12" t="s">
         <v>151</v>
-      </c>
-      <c r="D12" t="s">
-        <v>150</v>
-      </c>
-      <c r="E12" t="s">
-        <v>152</v>
       </c>
       <c r="F12" s="4">
         <v>1</v>
@@ -1250,24 +1250,24 @@
         <v>1.71</v>
       </c>
       <c r="I12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" t="s">
         <v>79</v>
       </c>
-      <c r="B13" t="s">
-        <v>80</v>
-      </c>
       <c r="C13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F13" s="4">
         <v>1</v>
@@ -1280,24 +1280,24 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" t="s">
         <v>89</v>
       </c>
-      <c r="B14" t="s">
-        <v>90</v>
-      </c>
       <c r="C14" t="s">
+        <v>152</v>
+      </c>
+      <c r="D14" t="s">
         <v>153</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>154</v>
-      </c>
-      <c r="E14" t="s">
-        <v>155</v>
       </c>
       <c r="F14" s="4">
         <v>1</v>
@@ -1310,24 +1310,24 @@
         <v>0.45</v>
       </c>
       <c r="I14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" t="s">
         <v>23</v>
-      </c>
-      <c r="E15" t="s">
-        <v>24</v>
       </c>
       <c r="F15" s="3">
         <v>1</v>
@@ -1340,24 +1340,24 @@
         <v>0.94</v>
       </c>
       <c r="I15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" t="s">
         <v>73</v>
       </c>
-      <c r="B16" t="s">
-        <v>74</v>
-      </c>
       <c r="C16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D16" t="s">
         <v>158</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>159</v>
-      </c>
-      <c r="E16" t="s">
-        <v>160</v>
       </c>
       <c r="F16" s="4">
         <v>1</v>
@@ -1370,24 +1370,24 @@
         <v>0.86</v>
       </c>
       <c r="I16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F17" s="4">
         <v>4</v>
@@ -1400,24 +1400,24 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D18" s="2">
         <v>788640001</v>
       </c>
       <c r="E18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F18" s="4">
         <v>2</v>
@@ -1430,24 +1430,24 @@
         <v>0.76</v>
       </c>
       <c r="I18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" t="s">
         <v>58</v>
       </c>
-      <c r="B19" t="s">
-        <v>95</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>59</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>60</v>
-      </c>
-      <c r="E19" t="s">
-        <v>61</v>
       </c>
       <c r="F19" s="3">
         <v>1</v>
@@ -1460,24 +1460,24 @@
         <v>0.5</v>
       </c>
       <c r="I19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" t="s">
         <v>63</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>64</v>
-      </c>
-      <c r="E20" t="s">
-        <v>65</v>
       </c>
       <c r="F20" s="3">
         <v>5</v>
@@ -1490,24 +1490,24 @@
         <v>1.9</v>
       </c>
       <c r="I20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" t="s">
         <v>67</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>68</v>
-      </c>
-      <c r="E21" t="s">
-        <v>69</v>
       </c>
       <c r="F21" s="3">
         <v>1</v>
@@ -1520,24 +1520,24 @@
         <v>0.7</v>
       </c>
       <c r="I21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" t="s">
         <v>110</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>111</v>
-      </c>
-      <c r="E22" t="s">
-        <v>112</v>
       </c>
       <c r="F22" s="3">
         <v>5</v>
@@ -1550,24 +1550,24 @@
         <v>2.35E-2</v>
       </c>
       <c r="I22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C23" t="s">
+        <v>121</v>
+      </c>
+      <c r="D23" t="s">
         <v>122</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>123</v>
-      </c>
-      <c r="E23" t="s">
-        <v>124</v>
       </c>
       <c r="F23" s="3">
         <v>1</v>
@@ -1580,24 +1580,24 @@
         <v>0.4</v>
       </c>
       <c r="I23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C24" t="s">
+        <v>125</v>
+      </c>
+      <c r="D24" t="s">
         <v>126</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>127</v>
-      </c>
-      <c r="E24" t="s">
-        <v>128</v>
       </c>
       <c r="F24" s="3">
         <v>1</v>
@@ -1610,24 +1610,24 @@
         <v>0.4</v>
       </c>
       <c r="I24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C25" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25" t="s">
         <v>114</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>115</v>
-      </c>
-      <c r="E25" t="s">
-        <v>116</v>
       </c>
       <c r="F25" s="3">
         <v>3</v>
@@ -1640,24 +1640,24 @@
         <v>1.4100000000000001E-2</v>
       </c>
       <c r="I25" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" t="s">
         <v>35</v>
       </c>
-      <c r="B26" t="s">
-        <v>36</v>
-      </c>
       <c r="C26" t="s">
+        <v>117</v>
+      </c>
+      <c r="D26" t="s">
         <v>118</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>119</v>
-      </c>
-      <c r="E26" t="s">
-        <v>120</v>
       </c>
       <c r="F26" s="3">
         <v>2</v>
@@ -1670,24 +1670,24 @@
         <v>9.4000000000000004E-3</v>
       </c>
       <c r="I26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
         <v>17</v>
       </c>
       <c r="C27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" t="s">
         <v>45</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>46</v>
-      </c>
-      <c r="E27" t="s">
-        <v>47</v>
       </c>
       <c r="F27" s="3">
         <v>1</v>
@@ -1700,24 +1700,24 @@
         <v>5.51</v>
       </c>
       <c r="I27" t="s">
-        <v>18</v>
+        <v>172</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C28" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D28" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E28" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F28" s="4">
         <v>1</v>
@@ -1730,12 +1730,12 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="I28" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" t="s">
         <v>5</v>
@@ -1765,7 +1765,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" t="s">
         <v>13</v>
@@ -1790,7 +1790,7 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="I30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Revert to use older Op-Amp
</commit_message>
<xml_diff>
--- a/pcb/bom.xlsx
+++ b/pcb/bom.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sawaiz\OneDrive\projects\mppcSensorInterface\pcb\sensorBoard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sawaiz\Desktop\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -161,9 +161,6 @@
     <t xml:space="preserve"> THERMISTOR NTC 100KOHM 0.5% 0603</t>
   </si>
   <si>
-    <t>LED UV/NUV 380NM 200MW FLIPCHIP</t>
-  </si>
-  <si>
     <t>Decoupling/Low-Pass</t>
   </si>
   <si>
@@ -224,15 +221,6 @@
     <t>http://www.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=191776695&amp;uq=635931346694799446</t>
   </si>
   <si>
-    <t>L1F2-U380100002001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1416-1494-1-ND</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=191777383&amp;uq=635931346694829449</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=191775856&amp;uq=635931346694789445</t>
   </si>
   <si>
@@ -345,6 +333,18 @@
   </si>
   <si>
     <t>609-3140-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?keywords=160-1475-1-ND</t>
+  </si>
+  <si>
+    <t>LED GREEN CLEAR 0603 R/A SMD</t>
+  </si>
+  <si>
+    <t>LTST-S270GKT</t>
+  </si>
+  <si>
+    <t>160-1475-1-ND</t>
   </si>
 </sst>
 </file>
@@ -686,7 +686,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,19 +733,19 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F2" s="3">
         <v>4</v>
@@ -758,7 +758,7 @@
         <v>9.2399999999999996E-2</v>
       </c>
       <c r="I2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -772,10 +772,10 @@
         <v>32</v>
       </c>
       <c r="D3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" t="s">
         <v>52</v>
-      </c>
-      <c r="E3" t="s">
-        <v>53</v>
       </c>
       <c r="F3" s="4">
         <v>1</v>
@@ -788,7 +788,7 @@
         <v>7.1999999999999998E-3</v>
       </c>
       <c r="I3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -802,10 +802,10 @@
         <v>33</v>
       </c>
       <c r="D4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" t="s">
         <v>55</v>
-      </c>
-      <c r="E4" t="s">
-        <v>56</v>
       </c>
       <c r="F4" s="3">
         <v>1</v>
@@ -818,7 +818,7 @@
         <v>2.75E-2</v>
       </c>
       <c r="I4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -832,10 +832,10 @@
         <v>35</v>
       </c>
       <c r="D5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" t="s">
         <v>58</v>
-      </c>
-      <c r="E5" t="s">
-        <v>59</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -848,7 +848,7 @@
         <v>1.4E-2</v>
       </c>
       <c r="I5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -862,10 +862,10 @@
         <v>34</v>
       </c>
       <c r="D6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" t="s">
         <v>61</v>
-      </c>
-      <c r="E6" t="s">
-        <v>62</v>
       </c>
       <c r="F6" s="3">
         <v>1</v>
@@ -878,7 +878,7 @@
         <v>6.5600000000000006E-2</v>
       </c>
       <c r="I6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -892,10 +892,10 @@
         <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F7" s="3">
         <v>1</v>
@@ -908,7 +908,7 @@
         <v>22</v>
       </c>
       <c r="I7" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -919,26 +919,26 @@
         <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>103</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>104</v>
       </c>
       <c r="E8" t="s">
-        <v>66</v>
+        <v>105</v>
       </c>
       <c r="F8" s="4">
         <v>1</v>
       </c>
       <c r="G8" s="5">
-        <v>4.242</v>
+        <v>0.11219999999999999</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
-        <v>4.242</v>
+        <v>0.11219999999999999</v>
       </c>
       <c r="I8" t="s">
-        <v>67</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -946,16 +946,16 @@
         <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C9" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D9" s="2">
         <v>788640001</v>
       </c>
       <c r="E9" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F9" s="4">
         <v>2</v>
@@ -968,12 +968,12 @@
         <v>0.50939999999999996</v>
       </c>
       <c r="I9" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
         <v>28</v>
@@ -982,10 +982,10 @@
         <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E10" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F10" s="4">
         <v>1</v>
@@ -998,7 +998,7 @@
         <v>0.1333</v>
       </c>
       <c r="I10" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1012,10 +1012,10 @@
         <v>43</v>
       </c>
       <c r="D11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E11" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F11" s="4">
         <v>1</v>
@@ -1028,7 +1028,7 @@
         <v>0.31269999999999998</v>
       </c>
       <c r="I11" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1042,10 +1042,10 @@
         <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E12" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F12" s="4">
         <v>1</v>
@@ -1058,12 +1058,12 @@
         <v>1.66E-2</v>
       </c>
       <c r="I12" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
         <v>27</v>
@@ -1072,10 +1072,10 @@
         <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F13" s="4">
         <v>2</v>
@@ -1088,7 +1088,7 @@
         <v>0.2666</v>
       </c>
       <c r="I13" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1102,10 +1102,10 @@
         <v>38</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E14" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F14" s="4">
         <v>1</v>
@@ -1118,7 +1118,7 @@
         <v>1.6199999999999999E-2</v>
       </c>
       <c r="I14" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1132,10 +1132,10 @@
         <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E15" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F15" s="3">
         <v>1</v>
@@ -1148,7 +1148,7 @@
         <v>1.66E-2</v>
       </c>
       <c r="I15" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1162,10 +1162,10 @@
         <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E16" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F16" s="3">
         <v>1</v>
@@ -1178,24 +1178,24 @@
         <v>8.8510000000000009</v>
       </c>
       <c r="I16" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" t="s">
         <v>96</v>
-      </c>
-      <c r="C17" t="s">
-        <v>99</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E17" t="s">
-        <v>100</v>
       </c>
       <c r="F17" s="3">
         <v>1</v>
@@ -1208,24 +1208,24 @@
         <v>0.58199999999999996</v>
       </c>
       <c r="I17" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B18" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C18" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D18" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E18" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F18" s="3">
         <v>1</v>
@@ -1238,7 +1238,7 @@
         <v>1.0880000000000001</v>
       </c>
       <c r="I18" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
BOM fixed, REF-DES cahnged for led
</commit_message>
<xml_diff>
--- a/pcb/bom.xlsx
+++ b/pcb/bom.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawaiz\OneDrive\projects\mppcSensor\pcb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawaiz\oneDrive\projects\mppcSensor\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="5475"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="bom" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">bom!$A$1:$I$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="71">
   <si>
     <t>QTY</t>
   </si>
@@ -83,9 +83,6 @@
     <t>MPPC</t>
   </si>
   <si>
-    <t>1.3x1.3mm MPPC</t>
-  </si>
-  <si>
     <t>Led</t>
   </si>
   <si>
@@ -116,18 +113,12 @@
     <t>490-10475-1-ND</t>
   </si>
   <si>
-    <t>S13360-1375PE</t>
-  </si>
-  <si>
     <t>NCP18WF104D03RB</t>
   </si>
   <si>
     <t>490-11811-1-ND</t>
   </si>
   <si>
-    <t>http://www.hamamatsu.com/eu/en/product/new/S13360-1375PE/index.html</t>
-  </si>
-  <si>
     <t>Spring Connector</t>
   </si>
   <si>
@@ -140,36 +131,9 @@
     <t>J3</t>
   </si>
   <si>
-    <t>J3-F</t>
-  </si>
-  <si>
     <t>Ouptut Header</t>
   </si>
   <si>
-    <t>Output Header Jack</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CONN IDC SOCKET 8POS 2MM GOLD</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CONN HEADER 2MM DUAL SMD 8POS</t>
-  </si>
-  <si>
-    <t>S6009-04-ND</t>
-  </si>
-  <si>
-    <t>NRPN042MAMS-RC</t>
-  </si>
-  <si>
-    <t>89361-708LF</t>
-  </si>
-  <si>
-    <t>609-3140-ND</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-search/en?keywords=160-1475-1-ND</t>
-  </si>
-  <si>
     <t>LED GREEN CLEAR 0603 R/A SMD</t>
   </si>
   <si>
@@ -242,39 +206,6 @@
     <t>RC0402JR-0710RL</t>
   </si>
   <si>
-    <t>http://www.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=193599532&amp;uq=635957905848336140</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=193543977&amp;uq=635957905848296132</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=193599527&amp;uq=635957905848326138</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=193546069&amp;uq=635957905848326138</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=193545736&amp;uq=635957905848316136</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=193544331&amp;uq=635957905848306134</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=193544046&amp;uq=635957905848296132</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=193543958&amp;uq=635957905848286130</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=193544010&amp;uq=635957905848296132</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=193544467&amp;uq=635957905848306134</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=193546846&amp;uq=635957905848326138</t>
-  </si>
-  <si>
     <t>CAP CER 0.047UF 50V X7R 0402</t>
   </si>
   <si>
@@ -284,9 +215,6 @@
     <t>490-10702-1-ND</t>
   </si>
   <si>
-    <t>https://www.digikey.com/product-search/en?keywords=490-10018-1-ND</t>
-  </si>
-  <si>
     <t>GRM155R61E105MA12D</t>
   </si>
   <si>
@@ -294,6 +222,24 @@
   </si>
   <si>
     <t>490-10018-1-ND</t>
+  </si>
+  <si>
+    <t>2.0mmx2.0mm MPPC</t>
+  </si>
+  <si>
+    <t>S13360-2050VE</t>
+  </si>
+  <si>
+    <t>http://www.hamamatsu.com/us/en/community/mppc/4400/S13360-2050VE/index.html</t>
+  </si>
+  <si>
+    <t>98424-F52-08ALF</t>
+  </si>
+  <si>
+    <t>MINITEK</t>
+  </si>
+  <si>
+    <t>609-5175-1-ND</t>
   </si>
 </sst>
 </file>
@@ -301,10 +247,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00000_);_(&quot;$&quot;* \(#,##0.00000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00000_);_(&quot;$&quot;* \(#,##0.00000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,12 +264,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -345,21 +285,15 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -454,6 +388,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -489,6 +440,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -644,7 +612,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,7 +625,7 @@
     <col min="6" max="6" width="8.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.7109375" customWidth="1"/>
+    <col min="9" max="9" width="78.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -691,19 +659,19 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="E2" t="s">
-        <v>88</v>
+        <v>63</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="F2" s="4">
         <v>1</v>
@@ -712,28 +680,29 @@
         <v>3.2500000000000001E-2</v>
       </c>
       <c r="H2" s="1">
-        <f t="shared" ref="H2:H15" si="0">G2*F2</f>
+        <f>G2*F2</f>
         <v>3.2500000000000001E-2</v>
       </c>
-      <c r="I2" t="s">
-        <v>85</v>
+      <c r="I2" t="str">
+        <f>CONCATENATE("http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=",E2)</f>
+        <v>http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=490-10018-1-ND</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E3" t="s">
-        <v>84</v>
+        <v>59</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="F3" s="3">
         <v>1</v>
@@ -742,11 +711,12 @@
         <v>1.32E-2</v>
       </c>
       <c r="H3" s="1">
-        <f t="shared" si="0"/>
+        <f>G3*F3</f>
         <v>1.32E-2</v>
       </c>
-      <c r="I3" t="s">
-        <v>81</v>
+      <c r="I3" t="str">
+        <f>CONCATENATE("http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=",E3)</f>
+        <v>http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=490-10702-1-ND</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -757,13 +727,13 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
       </c>
       <c r="F4" s="3">
         <v>1</v>
@@ -772,11 +742,12 @@
         <v>1.4E-2</v>
       </c>
       <c r="H4" s="1">
-        <f t="shared" si="0"/>
+        <f>G4*F4</f>
         <v>1.4E-2</v>
       </c>
-      <c r="I4" t="s">
-        <v>79</v>
+      <c r="I4" t="str">
+        <f>CONCATENATE("http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=",E4)</f>
+        <v>http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=1276-1182-1-ND</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -787,13 +758,13 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -802,11 +773,12 @@
         <v>6.5600000000000006E-2</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" si="0"/>
+        <f>G5*F5</f>
         <v>6.5600000000000006E-2</v>
       </c>
-      <c r="I5" t="s">
-        <v>80</v>
+      <c r="I5" t="str">
+        <f>CONCATENATE("http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=",E5)</f>
+        <v>http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=490-10475-1-ND</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -817,13 +789,13 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" t="s">
-        <v>29</v>
+        <v>65</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="F6" s="3">
         <v>1</v>
@@ -832,11 +804,11 @@
         <v>22</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" si="0"/>
+        <f>G6*F6</f>
         <v>22</v>
       </c>
       <c r="I6" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -844,16 +816,16 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" t="s">
-        <v>49</v>
+        <v>35</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="F7" s="4">
         <v>1</v>
@@ -862,28 +834,29 @@
         <v>0.11219999999999999</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="0"/>
+        <f>G7*F7</f>
         <v>0.11219999999999999</v>
       </c>
-      <c r="I7" t="s">
-        <v>46</v>
+      <c r="I7" t="str">
+        <f>CONCATENATE("http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=",E7)</f>
+        <v>http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=160-1475-1-ND</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D8" s="2">
         <v>788640001</v>
       </c>
-      <c r="E8" t="s">
-        <v>35</v>
+      <c r="E8" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="F8" s="4">
         <v>2</v>
@@ -892,28 +865,29 @@
         <v>0.25469999999999998</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="0"/>
+        <f>G8*F8</f>
         <v>0.50939999999999996</v>
       </c>
-      <c r="I8" t="s">
-        <v>78</v>
+      <c r="I8" t="str">
+        <f>CONCATENATE("http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=",E8)</f>
+        <v>http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=WM11203CT-ND</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" t="s">
-        <v>68</v>
+        <v>57</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="F9" s="4">
         <v>2</v>
@@ -922,11 +896,12 @@
         <v>4.7000000000000002E-3</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" si="0"/>
+        <f>G9*F9</f>
         <v>9.4000000000000004E-3</v>
       </c>
-      <c r="I9" t="s">
-        <v>71</v>
+      <c r="I9" t="str">
+        <f>CONCATENATE("http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=",E9)</f>
+        <v>http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=311-10JRCT-ND</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -934,16 +909,16 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" t="s">
-        <v>31</v>
+        <v>23</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="F10" s="4">
         <v>1</v>
@@ -952,28 +927,29 @@
         <v>0.31269999999999998</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" si="0"/>
+        <f>G10*F10</f>
         <v>0.31269999999999998</v>
       </c>
-      <c r="I10" t="s">
-        <v>72</v>
+      <c r="I10" t="str">
+        <f>CONCATENATE("http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=",E10)</f>
+        <v>http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=490-11811-1-ND</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="C11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" t="s">
-        <v>67</v>
       </c>
       <c r="F11" s="4">
         <v>3</v>
@@ -982,28 +958,29 @@
         <v>4.7000000000000002E-3</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" si="0"/>
+        <f>G11*F11</f>
         <v>1.4100000000000001E-2</v>
       </c>
-      <c r="I11" t="s">
-        <v>73</v>
+      <c r="I11" t="str">
+        <f>CONCATENATE("http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=",E11)</f>
+        <v>http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=311-51JRCT-ND</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" t="s">
-        <v>64</v>
+        <v>50</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="F12" s="4">
         <v>2</v>
@@ -1012,11 +989,12 @@
         <v>0.12759999999999999</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="0"/>
+        <f>G12*F12</f>
         <v>0.25519999999999998</v>
       </c>
-      <c r="I12" t="s">
-        <v>74</v>
+      <c r="I12" t="str">
+        <f>CONCATENATE("http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=",E12)</f>
+        <v>http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=YAG1386CT-ND</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1027,13 +1005,13 @@
         <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" t="s">
-        <v>61</v>
+        <v>47</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="F13" s="3">
         <v>1</v>
@@ -1042,72 +1020,49 @@
         <v>3.7446000000000002</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="0"/>
+        <f>G13*F13</f>
         <v>3.7446000000000002</v>
       </c>
-      <c r="I13" t="s">
-        <v>75</v>
+      <c r="I13" t="str">
+        <f>CONCATENATE("http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=",E13)</f>
+        <v>http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=296-14776-1-ND</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" t="s">
-        <v>42</v>
+        <v>69</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="F14" s="3">
         <v>1</v>
       </c>
       <c r="G14" s="5">
-        <v>0.58199999999999996</v>
+        <v>1.04</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" si="0"/>
-        <v>0.58199999999999996</v>
-      </c>
-      <c r="I14" t="s">
-        <v>76</v>
+        <f>G14*F14</f>
+        <v>1.04</v>
+      </c>
+      <c r="I14" t="str">
+        <f>CONCATENATE("http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=",E14)</f>
+        <v>http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=609-5175-1-ND</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="3">
-        <v>1</v>
-      </c>
-      <c r="G15" s="5">
-        <v>1.0880000000000001</v>
-      </c>
-      <c r="H15" s="1">
-        <f t="shared" si="0"/>
-        <v>1.0880000000000001</v>
-      </c>
-      <c r="I15" t="s">
-        <v>77</v>
-      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F16" s="3"/>

</xml_diff>